<commit_message>
comitting to sync with Dirk
</commit_message>
<xml_diff>
--- a/PCB_rev_A2/Replicape_BOM_rev1.xlsx
+++ b/PCB_rev_A2/Replicape_BOM_rev1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
   <si>
     <t>Digikey Part nr.</t>
   </si>
@@ -266,12 +266,6 @@
     <t>C14, C15, C16</t>
   </si>
   <si>
-    <t>311-1375-1-ND</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 25V Y5V 0402</t>
-  </si>
-  <si>
     <t>311-1363-1-ND</t>
   </si>
   <si>
@@ -290,12 +284,6 @@
     <t>C1, C3, C5, C7, C9</t>
   </si>
   <si>
-    <t>S2012E-13-ND</t>
-  </si>
-  <si>
-    <t>CONN HEADER .100 DUAL STR 26POS</t>
-  </si>
-  <si>
     <t>SAM1204-23-ND</t>
   </si>
   <si>
@@ -305,12 +293,6 @@
     <t>P9-EXPANSION_A, P8-EXPANSION_A</t>
   </si>
   <si>
-    <t>SAM1204-10-ND</t>
-  </si>
-  <si>
-    <t>CONN RCPT .100" 20POS DUAL TIN</t>
-  </si>
-  <si>
     <t>296-6604-1-ND</t>
   </si>
   <si>
@@ -335,7 +317,7 @@
     <t>Optional:</t>
   </si>
   <si>
-    <t>KIT BEAGLEBONE DEV</t>
+    <t>KIT BEAGLEBONE BLACK DEV</t>
   </si>
   <si>
     <t>None</t>
@@ -384,7 +366,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,12 +383,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="0000FF00"/>
         <bgColor rgb="0023FF23"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00993300"/>
       </patternFill>
     </fill>
     <fill>
@@ -450,7 +426,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -469,15 +445,11 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -559,17 +531,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+      <selection activeCell="B40" activeCellId="0" pane="topLeft" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.121568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.3254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7882352941176"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -1400,306 +1372,217 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="9" t="n">
+      <c r="C27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="E27" s="4" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="F27" s="4" t="n">
+        <f aca="false">D27*E27</f>
+        <v>0.861</v>
+      </c>
+      <c r="G27" s="4" t="n">
+        <f aca="false">D27*500</f>
+        <v>10500</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>0.0102</v>
+      </c>
+      <c r="I27" s="4" t="n">
+        <f aca="false">G27*H27</f>
+        <v>107.1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
+      <c r="A28" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2" t="n">
         <v>0.1</v>
       </c>
-      <c r="F27" s="9" t="n">
-        <f aca="false">D27*E27</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="9" t="n">
-        <f aca="false">D27*500</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="9" t="n">
-        <v>0.00405</v>
-      </c>
-      <c r="I27" s="9" t="n">
-        <f aca="false">G27*H27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
-      <c r="A28" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="E28" s="4" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="2" t="n">
         <f aca="false">D28*E28</f>
-        <v>0.861</v>
-      </c>
-      <c r="G28" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="2" t="n">
         <f aca="false">D28*500</f>
-        <v>10500</v>
-      </c>
-      <c r="H28" s="4" t="n">
-        <v>0.0102</v>
-      </c>
-      <c r="I28" s="4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0.00648</v>
+      </c>
+      <c r="I28" s="2" t="n">
         <f aca="false">G28*H28</f>
-        <v>107.1</v>
+        <v>16.2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
-      <c r="A29" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F29" s="2" t="n">
-        <f aca="false">D29*E29</f>
-        <v>0.5</v>
-      </c>
-      <c r="G29" s="2" t="n">
-        <f aca="false">D29*500</f>
-        <v>2500</v>
-      </c>
-      <c r="H29" s="2" t="n">
-        <v>0.00648</v>
-      </c>
-      <c r="I29" s="2" t="n">
-        <f aca="false">G29*H29</f>
-        <v>16.2</v>
+      <c r="C29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>4.72</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <f aca="false">E29*D29</f>
+        <v>9.44</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H29" s="3" t="n">
+        <v>2.7492</v>
+      </c>
+      <c r="I29" s="4" t="n">
+        <f aca="false">H29*G29</f>
+        <v>2749.2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
-      <c r="A30" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="9" t="n">
-        <v>1.2</v>
+      <c r="B30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8" t="n">
+        <v>0.41</v>
       </c>
       <c r="F30" s="9" t="n">
-        <f aca="false">D30*E30</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="9" t="n">
-        <f aca="false">D30*500</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="9" t="n">
-        <v>0.69894</v>
+        <f aca="false">E30*D30</f>
+        <v>0.41</v>
+      </c>
+      <c r="G30" s="8" t="n">
+        <v>500</v>
+      </c>
+      <c r="H30" s="8" t="n">
+        <v>0.15068</v>
       </c>
       <c r="I30" s="9" t="n">
-        <f aca="false">G30*H30</f>
-        <v>0</v>
+        <f aca="false">H30*G30</f>
+        <v>75.34</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
-      <c r="A31" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="A31" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E31" s="3" t="n">
-        <v>4.72</v>
-      </c>
-      <c r="F31" s="4" t="n">
+      <c r="B31" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="10" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="F31" s="9" t="n">
         <f aca="false">E31*D31</f>
-        <v>9.44</v>
-      </c>
-      <c r="G31" s="3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H31" s="3" t="n">
-        <v>2.7492</v>
-      </c>
-      <c r="I31" s="4" t="n">
+        <v>0.81</v>
+      </c>
+      <c r="G31" s="10" t="n">
+        <v>500</v>
+      </c>
+      <c r="H31" s="10" t="n">
+        <v>0.33496</v>
+      </c>
+      <c r="I31" s="9" t="n">
         <f aca="false">H31*G31</f>
-        <v>2749.2</v>
+        <v>167.48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="8" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="F32" s="9" t="n">
-        <f aca="false">E32*D32</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="8" t="n">
-        <v>1.5377</v>
-      </c>
-      <c r="I32" s="9" t="n">
-        <f aca="false">H32*G32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
-      <c r="A33" s="6" t="s">
+      <c r="A32" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11" t="n">
+        <f aca="false">SUM(F2:F31)</f>
+        <v>92.793</v>
+      </c>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11" t="n">
+        <f aca="false">SUM(I2:I31)/500</f>
+        <v>44.23811</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="A34" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C33" s="7" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="7" t="n">
+      <c r="C35" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="10" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="F33" s="11" t="n">
-        <f aca="false">E33*D33</f>
-        <v>0.41</v>
-      </c>
-      <c r="G33" s="10" t="n">
-        <v>500</v>
-      </c>
-      <c r="H33" s="10" t="n">
-        <v>0.15068</v>
-      </c>
-      <c r="I33" s="11" t="n">
-        <f aca="false">H33*G33</f>
-        <v>75.34</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
-      <c r="A34" s="12" t="s">
+      <c r="E35" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="36">
+      <c r="A36" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="12" t="n">
+      <c r="D36" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E34" s="12" t="n">
-        <v>0.81</v>
-      </c>
-      <c r="F34" s="11" t="n">
-        <f aca="false">E34*D34</f>
-        <v>0.81</v>
-      </c>
-      <c r="G34" s="12" t="n">
-        <v>500</v>
-      </c>
-      <c r="H34" s="12" t="n">
-        <v>0.33496</v>
-      </c>
-      <c r="I34" s="11" t="n">
-        <f aca="false">H34*G34</f>
-        <v>167.48</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
-      <c r="A35" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13" t="n">
-        <f aca="false">SUM(F2:F34)</f>
-        <v>92.793</v>
-      </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13" t="n">
-        <f aca="false">SUM(I2:I34)/500</f>
-        <v>44.23811</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
-      <c r="A37" s="13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="38">
-      <c r="A38" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="39">
-      <c r="A39" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="0" t="n">
+      <c r="E36" s="0" t="n">
         <v>69.95</v>
       </c>
     </row>

</xml_diff>